<commit_message>
recuperando datos de planilla excel
</commit_message>
<xml_diff>
--- a/Final/dominio/formulas-bkp.xlsx
+++ b/Final/dominio/formulas-bkp.xlsx
@@ -1,68 +1,65 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="23715" windowHeight="10050"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Hoja1" state="show" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+  <si>
+    <t>tag</t>
+  </si>
   <si>
     <t>valor</t>
   </si>
   <si>
-    <t>funcion</t>
-  </si>
-  <si>
     <t>ref</t>
   </si>
   <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>attr</t>
+  </si>
+  <si>
+    <t>PM_IPA_FERMENTACION_PRESION</t>
+  </si>
+  <si>
+    <t>stroke</t>
+  </si>
+  <si>
+    <t>fill</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
     <t>PM_IPA_CENTRIFUGADO_MARCHA</t>
-  </si>
-  <si>
-    <t>PM_IPA_FERMENTACION_PRESION</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>=</t>
-  </si>
-  <si>
-    <t>stroke</t>
-  </si>
-  <si>
-    <t>fill</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>tag entrada</t>
-  </si>
-  <si>
-    <t>attr salida</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,21 +82,18 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -113,6 +107,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -407,126 +404,126 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="2" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="1"/>
-    <col min="4" max="4" width="18.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
     <col min="5" max="5" width="3" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="2"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>11</v>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <v>3.15</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="str">
+      <c r="D2" t="str">
         <f>IF(B2&gt;C2,"green","blue")</f>
-        <v>blue</v>
+        <v>green</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
+      <c r="A3" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>4</v>
+        <v>3.15</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="str">
+      <c r="D3" t="str">
         <f>IF(B3&gt;C3,"red","yellow")</f>
         <v>red</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
+      <c r="A4" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>2.8</v>
+        <v>3.15</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="str">
-        <f>IF(B4&gt;C4,"presion alta","presion normal")</f>
-        <v>presion normal</v>
+      <c r="D4" t="str">
+        <f>IF(B4&gt;C4,"red","yellow")</f>
+        <v>red</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="str">
-        <f>IF(B5=C5,"bomba en marcha","bomba parada")</f>
-        <v>bomba en marcha</v>
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" t="str">
+        <f>IF(B5=C5,"green","blue")</f>
+        <v>blue</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>